<commit_message>
predicciones redneuronal opcion F
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\probabilidades\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E3FE93-32D6-455B-B105-AE041453C3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="47">
   <si>
     <t>31</t>
   </si>
@@ -152,13 +158,16 @@
   </si>
   <si>
     <t>24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> al numero mas bajito repetido del balanceado, se le suma lo que  arroje  error del valor absoluto hacia arriba y hacia abajo, si no coinciede se pone el numero que sigue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,7 +231,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -232,7 +241,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -329,20 +380,16 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -630,14 +677,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53:J58"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
@@ -645,7 +692,7 @@
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>37</v>
       </c>
@@ -665,7 +712,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -680,7 +727,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>0</v>
       </c>
@@ -700,7 +747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>1</v>
       </c>
@@ -720,7 +767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>2</v>
       </c>
@@ -743,7 +790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>3</v>
       </c>
@@ -766,7 +813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>4</v>
       </c>
@@ -786,7 +833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>5</v>
       </c>
@@ -806,7 +853,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E9" s="2">
         <v>45813</v>
       </c>
@@ -818,7 +865,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>17</v>
       </c>
@@ -841,7 +888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>1</v>
       </c>
@@ -861,7 +908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>17</v>
       </c>
@@ -884,7 +931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>14</v>
       </c>
@@ -907,7 +954,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>11</v>
       </c>
@@ -927,7 +974,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>13</v>
       </c>
@@ -947,7 +994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E16" s="2">
         <v>45814</v>
       </c>
@@ -959,7 +1006,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>15</v>
       </c>
@@ -979,7 +1026,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>5</v>
       </c>
@@ -999,7 +1046,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>5</v>
       </c>
@@ -1019,7 +1066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>30</v>
       </c>
@@ -1059,7 +1106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>31</v>
       </c>
@@ -1079,12 +1126,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E23" s="2">
         <v>45831</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>39</v>
       </c>
@@ -1110,7 +1157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>16</v>
       </c>
@@ -1136,7 +1183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:13">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>13</v>
       </c>
@@ -1162,7 +1209,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>40</v>
       </c>
@@ -1188,7 +1235,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:13">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +1261,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>41</v>
       </c>
@@ -1240,12 +1287,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:13">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E30" s="2">
         <v>45833</v>
       </c>
     </row>
-    <row r="31" spans="2:13">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>26</v>
       </c>
@@ -1271,7 +1318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0</v>
       </c>
@@ -1300,7 +1347,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:18">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0</v>
       </c>
@@ -1329,7 +1376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="2:18">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>1</v>
       </c>
@@ -1358,7 +1405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:18">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>2</v>
       </c>
@@ -1387,7 +1434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:18">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>9</v>
       </c>
@@ -1416,7 +1463,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:18">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>20</v>
       </c>
@@ -1424,7 +1471,7 @@
         <v>45845</v>
       </c>
     </row>
-    <row r="38" spans="2:18">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
         <v>36</v>
       </c>
@@ -1462,7 +1509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:18">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
         <v>1</v>
       </c>
@@ -1500,7 +1547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:18">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>45</v>
       </c>
@@ -1538,7 +1585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="2:18">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
         <v>45</v>
       </c>
@@ -1576,7 +1623,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="2:18">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>5</v>
       </c>
@@ -1614,7 +1661,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="2:18">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>24</v>
       </c>
@@ -1652,7 +1699,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="2:18">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E45" s="2">
         <v>45847</v>
       </c>
@@ -1663,7 +1710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:18">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
         <v>25</v>
       </c>
@@ -1686,7 +1733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="2:18">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>41</v>
       </c>
@@ -1709,7 +1756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="2:18">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>16</v>
       </c>
@@ -1732,7 +1779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="5:16">
+    <row r="49" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
         <v>36</v>
       </c>
@@ -1755,7 +1802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="5:16">
+    <row r="50" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
         <v>1</v>
       </c>
@@ -1778,7 +1825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="5:16">
+    <row r="51" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
         <v>40</v>
       </c>
@@ -1795,12 +1842,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="5:16">
+    <row r="52" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E52" s="2">
         <v>45851</v>
       </c>
     </row>
-    <row r="53" spans="5:16">
+    <row r="53" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
         <v>42</v>
       </c>
@@ -1817,7 +1864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="5:16">
+    <row r="54" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
         <v>6</v>
       </c>
@@ -1834,7 +1881,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="5:16">
+    <row r="55" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
         <v>23</v>
       </c>
@@ -1851,7 +1898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="5:16">
+    <row r="56" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
         <v>8</v>
       </c>
@@ -1868,7 +1915,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="5:16">
+    <row r="57" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
         <v>25</v>
       </c>
@@ -1885,7 +1932,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="5:16">
+    <row r="58" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
         <v>31</v>
       </c>
@@ -1902,34 +1949,555 @@
         <v>41</v>
       </c>
     </row>
+    <row r="59" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E59" s="2">
+        <v>45921</v>
+      </c>
+    </row>
+    <row r="60" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" t="s">
+        <v>18</v>
+      </c>
+      <c r="I60" t="s">
+        <v>8</v>
+      </c>
+      <c r="J60" t="s">
+        <v>44</v>
+      </c>
+      <c r="L60" s="4">
+        <v>7</v>
+      </c>
+      <c r="M60">
+        <v>18</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" t="s">
+        <v>19</v>
+      </c>
+      <c r="I61" t="s">
+        <v>4</v>
+      </c>
+      <c r="J61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L61">
+        <v>11</v>
+      </c>
+      <c r="M61">
+        <v>6</v>
+      </c>
+      <c r="N61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>40</v>
+      </c>
+      <c r="G62" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" t="s">
+        <v>39</v>
+      </c>
+      <c r="I62" t="s">
+        <v>31</v>
+      </c>
+      <c r="J62" t="s">
+        <v>22</v>
+      </c>
+      <c r="L62" s="4">
+        <v>19</v>
+      </c>
+      <c r="M62" t="s">
+        <v>4</v>
+      </c>
+      <c r="N62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" t="s">
+        <v>27</v>
+      </c>
+      <c r="I63" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" t="s">
+        <v>6</v>
+      </c>
+      <c r="L63" s="4">
+        <v>23</v>
+      </c>
+      <c r="M63">
+        <v>24</v>
+      </c>
+      <c r="N63">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>31</v>
+      </c>
+      <c r="G64" t="s">
+        <v>45</v>
+      </c>
+      <c r="H64" t="s">
+        <v>6</v>
+      </c>
+      <c r="I64" t="s">
+        <v>45</v>
+      </c>
+      <c r="J64" t="s">
+        <v>3</v>
+      </c>
+      <c r="L64" s="4">
+        <v>25</v>
+      </c>
+      <c r="M64">
+        <v>31</v>
+      </c>
+      <c r="N64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>40</v>
+      </c>
+      <c r="G65" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" t="s">
+        <v>18</v>
+      </c>
+      <c r="I65" t="s">
+        <v>8</v>
+      </c>
+      <c r="J65" t="s">
+        <v>25</v>
+      </c>
+      <c r="L65">
+        <v>35</v>
+      </c>
+      <c r="M65">
+        <v>30</v>
+      </c>
+      <c r="N65">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E66" s="2">
+        <v>45923</v>
+      </c>
+    </row>
+    <row r="67" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>16</v>
+      </c>
+      <c r="G67" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" t="s">
+        <v>3</v>
+      </c>
+      <c r="I67" t="s">
+        <v>4</v>
+      </c>
+      <c r="J67" t="s">
+        <v>44</v>
+      </c>
+      <c r="L67" s="4">
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>1</v>
+      </c>
+      <c r="N67" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>26</v>
+      </c>
+      <c r="G68" t="s">
+        <v>10</v>
+      </c>
+      <c r="H68" t="s">
+        <v>31</v>
+      </c>
+      <c r="I68" t="s">
+        <v>8</v>
+      </c>
+      <c r="J68" t="s">
+        <v>13</v>
+      </c>
+      <c r="L68" s="4">
+        <v>6</v>
+      </c>
+      <c r="M68">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>24</v>
+      </c>
+      <c r="G69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" t="s">
+        <v>19</v>
+      </c>
+      <c r="I69" t="s">
+        <v>8</v>
+      </c>
+      <c r="J69" t="s">
+        <v>25</v>
+      </c>
+      <c r="L69" s="4">
+        <v>7</v>
+      </c>
+      <c r="M69">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>1</v>
+      </c>
+      <c r="G70" t="s">
+        <v>27</v>
+      </c>
+      <c r="H70" t="s">
+        <v>6</v>
+      </c>
+      <c r="I70" t="s">
+        <v>45</v>
+      </c>
+      <c r="J70" t="s">
+        <v>36</v>
+      </c>
+      <c r="L70" s="4">
+        <v>22</v>
+      </c>
+      <c r="M70">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>24</v>
+      </c>
+      <c r="G71" t="s">
+        <v>27</v>
+      </c>
+      <c r="H71" t="s">
+        <v>13</v>
+      </c>
+      <c r="I71" t="s">
+        <v>15</v>
+      </c>
+      <c r="J71" t="s">
+        <v>45</v>
+      </c>
+      <c r="L71" s="4">
+        <v>23</v>
+      </c>
+      <c r="M71">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>45</v>
+      </c>
+      <c r="H72" t="s">
+        <v>11</v>
+      </c>
+      <c r="I72" t="s">
+        <v>15</v>
+      </c>
+      <c r="J72" t="s">
+        <v>11</v>
+      </c>
+      <c r="L72" s="4">
+        <v>24</v>
+      </c>
+      <c r="M72">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E73" s="2">
+        <v>45925</v>
+      </c>
+      <c r="L73" s="2">
+        <v>45926</v>
+      </c>
+    </row>
+    <row r="74" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>31</v>
+      </c>
+      <c r="G74" t="s">
+        <v>25</v>
+      </c>
+      <c r="H74" t="s">
+        <v>26</v>
+      </c>
+      <c r="I74" t="s">
+        <v>27</v>
+      </c>
+      <c r="J74" t="s">
+        <v>15</v>
+      </c>
+      <c r="L74">
+        <v>15</v>
+      </c>
+      <c r="N74">
+        <v>19</v>
+      </c>
+      <c r="O74">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" t="s">
+        <v>27</v>
+      </c>
+      <c r="H75" t="s">
+        <v>27</v>
+      </c>
+      <c r="I75" t="s">
+        <v>31</v>
+      </c>
+      <c r="J75" t="s">
+        <v>26</v>
+      </c>
+      <c r="L75">
+        <v>16</v>
+      </c>
+      <c r="N75">
+        <v>23</v>
+      </c>
+      <c r="O75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>10</v>
+      </c>
+      <c r="G76" t="s">
+        <v>25</v>
+      </c>
+      <c r="H76" t="s">
+        <v>3</v>
+      </c>
+      <c r="I76" t="s">
+        <v>45</v>
+      </c>
+      <c r="J76" t="s">
+        <v>43</v>
+      </c>
+      <c r="L76">
+        <v>21</v>
+      </c>
+      <c r="N76">
+        <v>12</v>
+      </c>
+      <c r="O76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>27</v>
+      </c>
+      <c r="G77" t="s">
+        <v>27</v>
+      </c>
+      <c r="H77" t="s">
+        <v>6</v>
+      </c>
+      <c r="I77" t="s">
+        <v>15</v>
+      </c>
+      <c r="J77" t="s">
+        <v>13</v>
+      </c>
+      <c r="L77">
+        <v>24</v>
+      </c>
+      <c r="N77">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>19</v>
+      </c>
+      <c r="G78" t="s">
+        <v>25</v>
+      </c>
+      <c r="H78" t="s">
+        <v>0</v>
+      </c>
+      <c r="I78" t="s">
+        <v>31</v>
+      </c>
+      <c r="J78" t="s">
+        <v>4</v>
+      </c>
+      <c r="L78">
+        <v>26</v>
+      </c>
+      <c r="N78">
+        <v>33</v>
+      </c>
+      <c r="O78">
+        <v>12</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>23</v>
+      </c>
+      <c r="G79" t="s">
+        <v>31</v>
+      </c>
+      <c r="H79" t="s">
+        <v>25</v>
+      </c>
+      <c r="I79" t="s">
+        <v>25</v>
+      </c>
+      <c r="J79" t="s">
+        <v>3</v>
+      </c>
+      <c r="L79">
+        <v>36</v>
+      </c>
+      <c r="N79">
+        <v>7</v>
+      </c>
+      <c r="O79">
+        <v>19</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E80" s="2">
+        <v>45929</v>
+      </c>
+      <c r="O80">
+        <v>23</v>
+      </c>
+      <c r="P80">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O81">
+        <v>30</v>
+      </c>
+      <c r="P81">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O82">
+        <v>33</v>
+      </c>
+      <c r="P82">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O83">
+        <v>34</v>
+      </c>
+      <c r="P83">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O78:O83">
+    <sortCondition ref="O78:O83"/>
+  </sortState>
   <mergeCells count="3">
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="F16:J16"/>
   </mergeCells>
+  <conditionalFormatting sqref="F3:J8">
+    <cfRule type="uniqueValues" dxfId="11" priority="9"/>
+    <cfRule type="uniqueValues" dxfId="10" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F10:J15 L13 L10 F16">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:J8">
-    <cfRule type="uniqueValues" dxfId="7" priority="6"/>
-    <cfRule type="uniqueValues" dxfId="6" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:J22">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-    <cfRule type="uniqueValues" dxfId="3" priority="4"/>
+    <cfRule type="uniqueValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:J29">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F31:J36">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F38:J43">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F60:J65 M62">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31:J36">
+  <conditionalFormatting sqref="F67:J72">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:J43">
+  <conditionalFormatting sqref="F74:J79">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>